<commit_message>
Tabela com features das plataformas abaixo do grafico
</commit_message>
<xml_diff>
--- a/Sources/Dataverse Comparative Review/Comparative.xlsx
+++ b/Sources/Dataverse Comparative Review/Comparative.xlsx
@@ -1245,7 +1245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="296">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -1722,28 +1722,10 @@
     <t xml:space="preserve">Total # of published datasets as of July 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">15,325 data packages (average size of 573MB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,709 public projects</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total # of published files as of May 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">50,000+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"800,000+"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~191,837</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total # of public users as of May 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,916 (as of July 2016)</t>
   </si>
   <si>
     <t xml:space="preserve">Most popular subject tags</t>
@@ -1796,6 +1778,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bepress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic and domain-specific ontologies</t>
   </si>
   <si>
     <t xml:space="preserve">Use Case</t>
@@ -2991,7 +2976,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.14"/>
@@ -3043,14 +3028,14 @@
   <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+      <selection pane="bottomRight" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="74.42"/>
@@ -6267,7 +6252,7 @@
       <c r="P61" s="30"/>
       <c r="Q61" s="39"/>
     </row>
-    <row r="62" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="24"/>
       <c r="B62" s="17" t="s">
         <v>150</v>
@@ -6278,8 +6263,8 @@
       <c r="D62" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E62" s="41" t="s">
-        <v>151</v>
+      <c r="E62" s="41" t="n">
+        <v>15325</v>
       </c>
       <c r="F62" s="42" t="s">
         <v>40</v>
@@ -6287,9 +6272,8 @@
       <c r="G62" s="43" t="n">
         <v>21846</v>
       </c>
-      <c r="H62" s="21" t="str">
-        <f aca="false">HYPERLINK("https://easy.dans.knaw.nl/ui/?wicket:bookmarkablePage=:nl.knaw.dans.easy.web.search.pages.PublicSearchResultPage&amp;q=mendeley+data","1500+")</f>
-        <v>1500+</v>
+      <c r="H62" s="21" t="n">
+        <v>1500</v>
       </c>
       <c r="I62" s="44" t="n">
         <v>243</v>
@@ -6297,8 +6281,8 @@
       <c r="J62" s="45" t="n">
         <v>4397</v>
       </c>
-      <c r="K62" s="13" t="s">
-        <v>152</v>
+      <c r="K62" s="13" t="n">
+        <v>12709</v>
       </c>
       <c r="L62" s="10"/>
       <c r="M62" s="10"/>
@@ -6307,10 +6291,10 @@
       <c r="P62" s="10"/>
       <c r="Q62" s="11"/>
     </row>
-    <row r="63" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="24"/>
       <c r="B63" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C63" s="40" t="n">
         <v>426</v>
@@ -6318,11 +6302,11 @@
       <c r="D63" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E63" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="F63" s="35" t="s">
-        <v>155</v>
+      <c r="E63" s="46" t="n">
+        <v>50000</v>
+      </c>
+      <c r="F63" s="35" t="n">
+        <v>800000</v>
       </c>
       <c r="G63" s="43" t="n">
         <v>197844</v>
@@ -6333,8 +6317,8 @@
       <c r="I63" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J63" s="47" t="s">
-        <v>156</v>
+      <c r="J63" s="47" t="n">
+        <v>191837</v>
       </c>
       <c r="K63" s="48" t="n">
         <v>885531</v>
@@ -6344,15 +6328,17 @@
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
-      <c r="Q63" s="11"/>
-    </row>
-    <row r="64" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q63" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="24"/>
       <c r="B64" s="17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D64" s="35" t="s">
         <v>40</v>
@@ -6363,8 +6349,8 @@
       <c r="F64" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G64" s="10" t="s">
-        <v>158</v>
+      <c r="G64" s="10" t="n">
+        <v>13916</v>
       </c>
       <c r="H64" s="10" t="s">
         <v>40</v>
@@ -6383,86 +6369,92 @@
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
-      <c r="Q64" s="11"/>
-    </row>
-    <row r="65" customFormat="false" ht="112.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q64" s="46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="109.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="24"/>
       <c r="B65" s="17" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E65" s="35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F65" s="35" t="s">
         <v>40</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H65" s="10" t="s">
         <v>40</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J65" s="35" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="K65" s="13" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
-      <c r="Q65" s="11"/>
-    </row>
-    <row r="66" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q65" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="24"/>
       <c r="B66" s="17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E66" s="35" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F66" s="50" t="str">
         <f aca="false">HYPERLINK("http://www.abs.gov.au/ausstats/abs@.nsf/0/4AE1B46AE2048A28CA25741800044242?opendocument","Australian and New Zealand Standard Research Classification (ANZSRC), 2008")</f>
         <v>Australian and New Zealand Standard Research Classification (ANZSRC), 2008</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J66" s="35" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
-      <c r="Q66" s="11"/>
+      <c r="Q66" s="11" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="51"/>
@@ -6520,17 +6512,17 @@
       <c r="Q79" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77">
+  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77 Q64">
     <cfRule type="beginsWith" priority="2" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Yes" dxfId="0">
       <formula>LEFT(C1,LEN("Yes"))="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77">
+  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77 Q64">
     <cfRule type="beginsWith" priority="3" operator="beginsWith" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="No" dxfId="1">
       <formula>LEFT(C1,LEN("No"))="No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77">
+  <conditionalFormatting sqref="C1:N1 N2:N77 P1:P77 O2:O77 C2:C13 D2:D9 E2:J45 K2:K13 L2:L44 M2:M41 D11:D45 C15:C45 K15:K45 C48:M59 C62:D77 G62:M77 F63:F77 E64:E77 Q64">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="unknown" dxfId="2">
       <formula>NOT(ISERROR(SEARCH("unknown",C1)))</formula>
     </cfRule>
@@ -6609,10 +6601,10 @@
   <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="45.16"/>
@@ -6628,7 +6620,7 @@
         <v>Median: 8 / 1st quartile: 4 / 3rd quartile: 12 / Mean: 8.70454545454546</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H1" s="56"/>
       <c r="I1" s="56"/>
@@ -6644,22 +6636,22 @@
     </row>
     <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="59" t="s">
         <v>175</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>180</v>
       </c>
       <c r="G2" s="62" t="str">
         <f aca="false">HYPERLINK("https://rd-alliance.org/system/files/documents/Dissertation_UseCase_RepoPlat_1.docx","Dissertation")</f>
@@ -6712,10 +6704,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D3" s="66" t="n">
         <f aca="false">(5*COUNT(G3:Q3))-(SUM(G3:Q3))</f>
@@ -6758,13 +6750,13 @@
     </row>
     <row r="4" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="64" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D4" s="66" t="n">
         <f aca="false">(5*COUNT(G4:Q4))-(SUM(G4:Q4))</f>
@@ -6807,13 +6799,13 @@
     </row>
     <row r="5" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D5" s="66" t="n">
         <f aca="false">(5*COUNT(G5:Q5))-(SUM(G5:Q5))</f>
@@ -6850,13 +6842,13 @@
     </row>
     <row r="6" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C6" s="70" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D6" s="66" t="n">
         <f aca="false">(5*COUNT(G6:Q6))-(SUM(G6:Q6))</f>
@@ -6893,13 +6885,13 @@
     </row>
     <row r="7" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D7" s="66" t="n">
         <f aca="false">(5*COUNT(G7:Q7))-(SUM(G7:Q7))</f>
@@ -6936,13 +6928,13 @@
     </row>
     <row r="8" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D8" s="66" t="n">
         <f aca="false">(5*COUNT(G8:Q8))-(SUM(G8:Q8))</f>
@@ -6979,13 +6971,13 @@
     </row>
     <row r="9" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D9" s="66" t="n">
         <f aca="false">(5*COUNT(G9:Q9))-(SUM(G9:Q9))</f>
@@ -7022,13 +7014,13 @@
     </row>
     <row r="10" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" s="66" t="n">
         <f aca="false">(5*COUNT(G10:Q10))-(SUM(G10:Q10))</f>
@@ -7065,13 +7057,13 @@
     </row>
     <row r="11" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D11" s="66" t="n">
         <f aca="false">(5*COUNT(G11:Q11))-(SUM(G11:Q11))</f>
@@ -7106,13 +7098,13 @@
     </row>
     <row r="12" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D12" s="66" t="n">
         <f aca="false">(5*COUNT(G12:Q12))-(SUM(G12:Q12))</f>
@@ -7147,13 +7139,13 @@
     </row>
     <row r="13" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="64" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D13" s="66" t="n">
         <f aca="false">(5*COUNT(G13:Q13))-(SUM(G13:Q13))</f>
@@ -7191,10 +7183,10 @@
         <v>38</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D14" s="66" t="n">
         <f aca="false">(5*COUNT(G14:Q14))-(SUM(G14:Q14))</f>
@@ -7229,13 +7221,13 @@
     </row>
     <row r="15" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D15" s="66" t="n">
         <f aca="false">(5*COUNT(G15:Q15))-(SUM(G15:Q15))</f>
@@ -7270,13 +7262,13 @@
     </row>
     <row r="16" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D16" s="66" t="n">
         <f aca="false">(5*COUNT(G16:Q16))-(SUM(G16:Q16))</f>
@@ -7311,13 +7303,13 @@
     </row>
     <row r="17" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D17" s="66" t="n">
         <f aca="false">(5*COUNT(G17:Q17))-(SUM(G17:Q17))</f>
@@ -7352,13 +7344,13 @@
     </row>
     <row r="18" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D18" s="66" t="n">
         <f aca="false">(5*COUNT(G18:Q18))-(SUM(G18:Q18))</f>
@@ -7393,13 +7385,13 @@
     </row>
     <row r="19" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="64" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D19" s="66" t="n">
         <f aca="false">(5*COUNT(G19:Q19))-(SUM(G19:Q19))</f>
@@ -7434,13 +7426,13 @@
     </row>
     <row r="20" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="64" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D20" s="66" t="n">
         <f aca="false">(5*COUNT(G20:Q20))-(SUM(G20:Q20))</f>
@@ -7473,13 +7465,13 @@
     </row>
     <row r="21" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B21" s="70" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D21" s="66" t="n">
         <f aca="false">(5*COUNT(G21:Q21))-(SUM(G21:Q21))</f>
@@ -7512,13 +7504,13 @@
     </row>
     <row r="22" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="64" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D22" s="66" t="n">
         <f aca="false">(5*COUNT(G22:Q22))-(SUM(G22:Q22))</f>
@@ -7551,13 +7543,13 @@
     </row>
     <row r="23" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="64" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D23" s="66" t="n">
         <f aca="false">(5*COUNT(G23:Q23))-(SUM(G23:Q23))</f>
@@ -7590,13 +7582,13 @@
     </row>
     <row r="24" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D24" s="66" t="n">
         <f aca="false">(5*COUNT(G24:Q24))-(SUM(G24:Q24))</f>
@@ -7629,13 +7621,13 @@
     </row>
     <row r="25" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D25" s="66" t="n">
         <f aca="false">(5*COUNT(G25:Q25))-(SUM(G25:Q25))</f>
@@ -7668,13 +7660,13 @@
     </row>
     <row r="26" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B26" s="70" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C26" s="70" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D26" s="66" t="n">
         <f aca="false">(5*COUNT(G26:Q26))-(SUM(G26:Q26))</f>
@@ -7707,13 +7699,13 @@
     </row>
     <row r="27" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B27" s="70" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C27" s="70" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D27" s="66" t="n">
         <f aca="false">(5*COUNT(G27:Q27))-(SUM(G27:Q27))</f>
@@ -7746,10 +7738,10 @@
     </row>
     <row r="28" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="64" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="66" t="n">
@@ -7783,13 +7775,13 @@
     </row>
     <row r="29" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C29" s="70" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D29" s="66" t="n">
         <f aca="false">(5*COUNT(G29:Q29))-(SUM(G29:Q29))</f>
@@ -7822,13 +7814,13 @@
     </row>
     <row r="30" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B30" s="70" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C30" s="70" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D30" s="66" t="n">
         <f aca="false">(5*COUNT(G30:Q30))-(SUM(G30:Q30))</f>
@@ -7861,13 +7853,13 @@
     </row>
     <row r="31" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B31" s="70" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D31" s="66" t="n">
         <f aca="false">(5*COUNT(G31:Q31))-(SUM(G31:Q31))</f>
@@ -7897,13 +7889,13 @@
     </row>
     <row r="32" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="64" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B32" s="70" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C32" s="70" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D32" s="66" t="n">
         <f aca="false">(5*COUNT(G32:Q32))-(SUM(G32:Q32))</f>
@@ -7934,13 +7926,13 @@
     </row>
     <row r="33" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C33" s="71" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D33" s="66" t="n">
         <f aca="false">(5*COUNT(G33:Q33))-(SUM(G33:Q33))</f>
@@ -7971,13 +7963,13 @@
     </row>
     <row r="34" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B34" s="70" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C34" s="70" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D34" s="66" t="n">
         <f aca="false">(5*COUNT(G34:Q34))-(SUM(G34:Q34))</f>
@@ -8008,13 +8000,13 @@
     </row>
     <row r="35" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B35" s="70" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D35" s="66" t="n">
         <f aca="false">(5*COUNT(G35:Q35))-(SUM(G35:Q35))</f>
@@ -8045,13 +8037,13 @@
     </row>
     <row r="36" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B36" s="70" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D36" s="66" t="n">
         <f aca="false">(5*COUNT(G36:Q36))-(SUM(G36:Q36))</f>
@@ -8082,13 +8074,13 @@
     </row>
     <row r="37" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B37" s="70" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C37" s="70" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D37" s="66" t="n">
         <f aca="false">(5*COUNT(G37:Q37))-(SUM(G37:Q37))</f>
@@ -8119,13 +8111,13 @@
     </row>
     <row r="38" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C38" s="70" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D38" s="66" t="n">
         <f aca="false">(5*COUNT(G38:Q38))-(SUM(G38:Q38))</f>
@@ -8156,13 +8148,13 @@
     </row>
     <row r="39" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C39" s="73" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D39" s="66" t="n">
         <f aca="false">(5*COUNT(G39:Q39))-(SUM(G39:Q39))</f>
@@ -8193,13 +8185,13 @@
     </row>
     <row r="40" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D40" s="66" t="n">
         <f aca="false">(5*COUNT(G40:Q40))-(SUM(G40:Q40))</f>
@@ -8230,13 +8222,13 @@
     </row>
     <row r="41" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="64" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B41" s="70" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C41" s="70" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D41" s="66" t="n">
         <f aca="false">(5*COUNT(G41:Q41))-(SUM(G41:Q41))</f>
@@ -8270,10 +8262,10 @@
         <v>38</v>
       </c>
       <c r="B42" s="70" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C42" s="70" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D42" s="66" t="n">
         <f aca="false">(5*COUNT(G42:Q42))-(SUM(G42:Q42))</f>
@@ -8304,13 +8296,13 @@
     </row>
     <row r="43" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C43" s="65" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D43" s="66" t="n">
         <f aca="false">(5*COUNT(G43:Q43))-(SUM(G43:Q43))</f>
@@ -8341,13 +8333,13 @@
     </row>
     <row r="44" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B44" s="70" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C44" s="70" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D44" s="66" t="n">
         <f aca="false">(5*COUNT(G44:Q44))-(SUM(G44:Q44))</f>
@@ -8378,13 +8370,13 @@
     </row>
     <row r="45" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="64" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B45" s="70" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C45" s="70" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D45" s="66" t="n">
         <f aca="false">(5*COUNT(G45:Q45))-(SUM(G45:Q45))</f>
@@ -8415,13 +8407,13 @@
     </row>
     <row r="46" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C46" s="65" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D46" s="66" t="n">
         <f aca="false">(5*COUNT(G46:Q46))-(SUM(G46:Q46))</f>
@@ -8457,7 +8449,7 @@
       <c r="E47" s="61"/>
       <c r="F47" s="74"/>
       <c r="G47" s="75" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H47" s="75"/>
       <c r="I47" s="75"/>
@@ -8720,7 +8712,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -8729,10 +8721,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="76" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C1" s="77"/>
       <c r="D1" s="77"/>
@@ -8768,7 +8760,7 @@
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="79" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E2" s="77"/>
       <c r="F2" s="77"/>
@@ -8795,10 +8787,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="78" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B3" s="78" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C3" s="77"/>
       <c r="D3" s="77"/>
@@ -8830,7 +8822,7 @@
         <v>116</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C4" s="77"/>
       <c r="D4" s="77"/>
@@ -8862,7 +8854,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C5" s="77"/>
       <c r="D5" s="77"/>
@@ -8894,7 +8886,7 @@
         <v>141</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C6" s="77"/>
       <c r="D6" s="77"/>
@@ -8926,7 +8918,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C7" s="77"/>
       <c r="D7" s="77"/>
@@ -8955,10 +8947,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="78" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C8" s="77"/>
       <c r="D8" s="77"/>
@@ -8987,7 +8979,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="78" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B9" s="78" t="s">
         <v>27</v>
@@ -9022,7 +9014,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C10" s="77"/>
       <c r="D10" s="77"/>
@@ -9051,10 +9043,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="78" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C11" s="77"/>
       <c r="D11" s="77"/>
@@ -9083,10 +9075,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="78" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B12" s="76" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C12" s="77"/>
       <c r="D12" s="77"/>
@@ -9115,10 +9107,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="78" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B13" s="76" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C13" s="77"/>
       <c r="D13" s="77"/>
@@ -9150,7 +9142,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="78" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C14" s="77"/>
       <c r="D14" s="77"/>
@@ -9246,7 +9238,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="76" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="77"/>
@@ -9278,7 +9270,7 @@
         <v>81</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="77"/>
@@ -9406,7 +9398,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="76" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C22" s="77"/>
       <c r="D22" s="77"/>
@@ -9466,7 +9458,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="77"/>
       <c r="B24" s="76" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C24" s="77"/>
       <c r="D24" s="77"/>
@@ -9496,7 +9488,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="77"/>
       <c r="B25" s="76" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C25" s="77"/>
       <c r="D25" s="77"/>
@@ -9526,7 +9518,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="77"/>
       <c r="B26" s="76" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="77"/>
@@ -9598,410 +9590,410 @@
   </sheetPr>
   <dimension ref="A1:AT69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="64.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="64" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="64" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E1" s="64" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F1" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="H1" s="64" t="s">
-        <v>194</v>
-      </c>
       <c r="I1" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="J1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K1" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L1" s="64" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="M1" s="64" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="N1" s="64" t="s">
         <v>38</v>
       </c>
       <c r="O1" s="64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="P1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="Q1" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="R1" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="S1" s="64" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="U1" s="64" t="s">
+        <v>184</v>
+      </c>
+      <c r="V1" s="64" t="s">
+        <v>222</v>
+      </c>
+      <c r="W1" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="R1" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="S1" s="64" t="s">
-        <v>220</v>
-      </c>
-      <c r="T1" s="64" t="s">
-        <v>186</v>
-      </c>
-      <c r="U1" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="V1" s="64" t="s">
-        <v>227</v>
-      </c>
-      <c r="W1" s="64" t="s">
-        <v>183</v>
-      </c>
-      <c r="X1" s="64" t="s">
-        <v>194</v>
-      </c>
       <c r="Y1" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Z1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AA1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AB1" s="64" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AC1" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AD1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AE1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AF1" s="64" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AG1" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AH1" s="64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="AI1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AJ1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AK1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AL1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AM1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AN1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="AO1" s="64" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="AP1" s="64" t="s">
         <v>38</v>
       </c>
       <c r="AQ1" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AR1" s="64" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AS1" s="64" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT1" s="64" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="203.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="65" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E2" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="70" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="H2" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="G2" s="70" t="s">
-        <v>192</v>
-      </c>
-      <c r="H2" s="71" t="s">
-        <v>195</v>
-      </c>
       <c r="I2" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="J2" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="K2" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="J2" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="K2" s="70" t="s">
+      <c r="L2" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="M2" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="N2" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="M2" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="N2" s="70" t="s">
-        <v>210</v>
-      </c>
       <c r="O2" s="71" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="P2" s="70" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="Q2" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="R2" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="S2" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="R2" s="70" t="s">
+      <c r="T2" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="S2" s="65" t="s">
-        <v>221</v>
-      </c>
-      <c r="T2" s="72" t="s">
+      <c r="U2" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="V2" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="U2" s="70" t="s">
+      <c r="W2" s="65" t="s">
         <v>225</v>
       </c>
-      <c r="V2" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="W2" s="65" t="s">
+      <c r="X2" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y2" s="65" t="s">
         <v>230</v>
       </c>
-      <c r="X2" s="65" t="s">
+      <c r="Z2" s="70" t="s">
         <v>232</v>
       </c>
-      <c r="Y2" s="65" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z2" s="70" t="s">
+      <c r="AA2" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB2" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="AA2" s="70" t="s">
-        <v>239</v>
-      </c>
-      <c r="AB2" s="65" t="s">
+      <c r="AC2" s="70" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD2" s="70" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE2" s="70" t="s">
         <v>242</v>
       </c>
-      <c r="AC2" s="70" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD2" s="70" t="s">
-        <v>245</v>
-      </c>
-      <c r="AE2" s="70" t="s">
-        <v>247</v>
-      </c>
       <c r="AF2" s="70" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="AG2" s="65" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="AH2" s="70" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="AI2" s="70" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="AJ2" s="70" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AK2" s="70" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="AL2" s="70" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="AM2" s="73" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AN2" s="71" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="AO2" s="70" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AP2" s="70" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AQ2" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR2" s="70" t="s">
+        <v>268</v>
+      </c>
+      <c r="AS2" s="70" t="s">
         <v>271</v>
       </c>
-      <c r="AR2" s="70" t="s">
+      <c r="AT2" s="70" t="s">
         <v>273</v>
-      </c>
-      <c r="AS2" s="70" t="s">
-        <v>276</v>
-      </c>
-      <c r="AT2" s="70" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="65" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E3" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="H3" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="70" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="71" t="s">
-        <v>196</v>
-      </c>
       <c r="I3" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="J3" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="K3" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="J3" s="70" t="s">
-        <v>202</v>
-      </c>
-      <c r="K3" s="70" t="s">
+      <c r="L3" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="M3" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="L3" s="65" t="s">
+      <c r="N3" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="M3" s="65" t="s">
-        <v>209</v>
-      </c>
-      <c r="N3" s="70" t="s">
-        <v>211</v>
-      </c>
       <c r="O3" s="71" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P3" s="70" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q3" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="R3" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="S3" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="R3" s="70" t="s">
+      <c r="T3" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="S3" s="65" t="s">
-        <v>222</v>
-      </c>
-      <c r="T3" s="72" t="s">
+      <c r="U3" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="V3" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="U3" s="70" t="s">
+      <c r="W3" s="65" t="s">
         <v>226</v>
       </c>
-      <c r="V3" s="73" t="s">
-        <v>229</v>
-      </c>
-      <c r="W3" s="65" t="s">
+      <c r="X3" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y3" s="70" t="s">
         <v>231</v>
       </c>
-      <c r="X3" s="73" t="s">
+      <c r="Z3" s="70" t="s">
         <v>233</v>
       </c>
-      <c r="Y3" s="70" t="s">
-        <v>236</v>
-      </c>
-      <c r="Z3" s="70" t="s">
-        <v>238</v>
-      </c>
       <c r="AA3" s="70" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AB3" s="65"/>
       <c r="AC3" s="70" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="AD3" s="70" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AE3" s="70" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="AF3" s="70" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AG3" s="71" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="AH3" s="70" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="AI3" s="70" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="AJ3" s="70" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AK3" s="70" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="AL3" s="70" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AM3" s="73" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="AN3" s="71" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AO3" s="70" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="AP3" s="70" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="AQ3" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="AR3" s="70" t="s">
+        <v>269</v>
+      </c>
+      <c r="AS3" s="70" t="s">
         <v>272</v>
       </c>
-      <c r="AR3" s="70" t="s">
+      <c r="AT3" s="65" t="s">
         <v>274</v>
-      </c>
-      <c r="AS3" s="70" t="s">
-        <v>277</v>
-      </c>
-      <c r="AT3" s="65" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10603,25 +10595,25 @@
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="24"/>
       <c r="B66" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="24"/>
       <c r="B67" s="17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="24"/>
       <c r="B68" s="17" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="24"/>
       <c r="B69" s="17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gráfico e tabela comparativa terminados
</commit_message>
<xml_diff>
--- a/Sources/Dataverse Comparative Review/Comparative.xlsx
+++ b/Sources/Dataverse Comparative Review/Comparative.xlsx
@@ -1245,7 +1245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="296">
   <si>
     <t xml:space="preserve">Information</t>
   </si>
@@ -2976,7 +2976,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.14"/>
@@ -3028,14 +3028,14 @@
   <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I54" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
-      <selection pane="bottomRight" activeCell="C63" activeCellId="0" sqref="C63"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="bottomRight" activeCell="Q63" activeCellId="0" sqref="Q63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="74.42"/>
@@ -6161,7 +6161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="38.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="24"/>
       <c r="B59" s="17" t="s">
         <v>146</v>
@@ -6289,7 +6289,9 @@
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
-      <c r="Q62" s="11"/>
+      <c r="Q62" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="14.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="24"/>
@@ -6604,7 +6606,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="45.16"/>
@@ -8712,7 +8714,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -9594,7 +9596,7 @@
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="64.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="64" t="s">

</xml_diff>